<commit_message>
Add the airplane mode by windows of LAN and WAN code.
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,6 +225,14 @@
   </si>
   <si>
     <t>已測兩千次 接近穩定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USM-210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWAN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -303,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -385,26 +393,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -441,6 +429,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -490,25 +491,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -526,13 +518,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -836,13 +837,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" style="2" bestFit="1" customWidth="1"/>
@@ -924,37 +927,37 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="15">
         <v>2000</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="15">
         <v>2000</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="15">
         <v>1999</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="15">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -991,34 +994,34 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>1000</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>1000</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23" t="s">
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1036,7 +1039,7 @@
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1071,7 +1074,7 @@
       <c r="J7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1094,7 +1097,7 @@
       <c r="F8" s="10">
         <v>186</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>814</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -1106,74 +1109,69 @@
       <c r="J8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="10">
         <v>1000</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="10">
         <v>1000</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="10">
         <v>979</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="22">
         <v>21</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3000</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2991</v>
-      </c>
-      <c r="G10" s="1">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="26">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="I10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1183,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
         <v>1500</v>
@@ -1192,10 +1190,10 @@
         <v>3000</v>
       </c>
       <c r="F11" s="1">
-        <v>2971</v>
-      </c>
-      <c r="G11" s="5">
-        <v>29</v>
+        <v>2991</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>25</v>
@@ -1204,40 +1202,39 @@
         <v>29</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <v>1500</v>
       </c>
-      <c r="E12" s="8">
-        <f>F12+G12</f>
-        <v>831</v>
-      </c>
-      <c r="F12" s="8">
-        <v>744</v>
-      </c>
-      <c r="G12" s="6">
-        <v>87</v>
+      <c r="E12" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2971</v>
+      </c>
+      <c r="G12" s="5">
+        <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1248,19 +1245,20 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
         <v>1500</v>
       </c>
       <c r="E13" s="8">
-        <v>309</v>
+        <f>F13+G13</f>
+        <v>831</v>
       </c>
       <c r="F13" s="8">
-        <v>263</v>
+        <v>744</v>
       </c>
       <c r="G13" s="6">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>25</v>
@@ -1269,41 +1267,73 @@
         <v>12</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1500</v>
+      </c>
+      <c r="E14" s="8">
+        <v>309</v>
+      </c>
+      <c r="F14" s="8">
+        <v>263</v>
+      </c>
+      <c r="G14" s="6">
+        <v>46</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D15" s="15">
         <v>10</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E15" s="15">
         <v>10</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F15" s="15">
         <v>10</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G15" s="15">
         <v>0</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H15" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K15" s="16" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the Summary Table and Statistics
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,10 +143,6 @@
     <t>20190904_095925</t>
   </si>
   <si>
-    <t>Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Local</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +229,22 @@
   </si>
   <si>
     <t>WWAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>airplane_wwan_windows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191106_041905</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWAN module crash at the 604 times</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,22 +530,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -839,9 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -861,13 +871,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -885,13 +895,13 @@
         <v>23</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -923,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -955,10 +965,10 @@
         <v>31</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -966,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -990,7 +1000,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1010,14 +1020,14 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="20"/>
       <c r="K5" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1034,13 +1044,13 @@
         <v>2000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1048,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -1066,16 +1076,16 @@
         <v>0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1107,10 +1117,10 @@
         <v>30</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>53</v>
+        <v>43</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1142,36 +1152,44 @@
         <v>28</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="26">
+      <c r="D10" s="25">
         <v>1000</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>1000</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28" t="s">
+      <c r="F10" s="25">
+        <v>603</v>
+      </c>
+      <c r="G10" s="26">
+        <v>397</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="12"/>
+      <c r="I10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1202,7 +1220,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1234,7 +1252,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1267,7 +1285,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1331,10 +1349,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the pxe sop for FULL auto installation
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,108 +143,136 @@
     <t>20190904_095925</t>
   </si>
   <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191017_051754</t>
+  </si>
+  <si>
+    <t>20191002_175658</t>
+  </si>
+  <si>
+    <t>20191009_084201</t>
+  </si>
+  <si>
+    <t>20191010_164358</t>
+  </si>
+  <si>
+    <t>20191009_043035</t>
+  </si>
+  <si>
+    <t>20190904_095925</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20190925_012123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20190920_224814</t>
+  </si>
+  <si>
+    <t>20191009_042845</t>
+  </si>
+  <si>
+    <t>MIO-2263</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android 8.1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191030_163844</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date and Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCM-8524</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Roaming 已穩定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(程式已完成) 等待可用設備</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同一隻程式跑不同設備 Fail Rate 不同</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>機器會自動休眠問題(所以先測 50 次)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已測兩千次 接近穩定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USM-210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>airplane_wwan_windows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191106_041905</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWAN module crash at the 604 times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PXE for Legacy x64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASMB-785</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pxe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Local</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191017_051754</t>
-  </si>
-  <si>
-    <t>20191002_175658</t>
-  </si>
-  <si>
-    <t>20191009_084201</t>
-  </si>
-  <si>
-    <t>20191010_164358</t>
-  </si>
-  <si>
-    <t>20191009_043035</t>
-  </si>
-  <si>
-    <t>20190904_095925</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20190925_012123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20190920_224814</t>
-  </si>
-  <si>
-    <t>20191009_042845</t>
-  </si>
-  <si>
-    <t>MIO-2263</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android 8.1.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191030_163844</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date and Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCM-8524</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Roaming 已穩定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(程式已完成) 等待可用設備</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同一隻程式跑不同設備 Fail Rate 不同</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>機器會自動休眠問題(所以先測 50 次)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已測兩千次 接近穩定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USM-210</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WWAN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tools</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>airplane_wwan_windows</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191106_041905</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WWAN module crash at the 604 times</t>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows 10 x64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019111_230256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,7 +488,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -503,9 +531,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,21 +543,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,6 +559,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -849,13 +883,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" style="2" bestFit="1" customWidth="1"/>
@@ -870,14 +904,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>33</v>
+      <c r="A1" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -895,17 +929,17 @@
         <v>23</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -933,50 +967,50 @@
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="14">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1999</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="15">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="15">
-        <v>2000</v>
-      </c>
-      <c r="F3" s="15">
-        <v>1999</v>
-      </c>
-      <c r="G3" s="15">
-        <v>1</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>54</v>
+      <c r="K3" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -1000,38 +1034,38 @@
         <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <v>1000</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <v>1000</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="20" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="20"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1044,21 +1078,21 @@
         <v>2000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="18" t="s">
-        <v>51</v>
+      <c r="K6" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -1076,20 +1110,20 @@
         <v>0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1107,7 +1141,7 @@
       <c r="F8" s="10">
         <v>186</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="19">
         <v>814</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -1117,14 +1151,14 @@
         <v>30</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1142,7 +1176,7 @@
       <c r="F9" s="10">
         <v>979</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="19">
         <v>21</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -1152,47 +1186,47 @@
         <v>28</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="28"/>
+        <v>34</v>
+      </c>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="25">
+      <c r="D10" s="21">
         <v>1000</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="21">
         <v>1000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="21">
         <v>603</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="22">
         <v>397</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="K10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1220,11 +1254,11 @@
         <v>29</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1252,11 +1286,11 @@
         <v>29</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1285,11 +1319,11 @@
         <v>12</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1321,38 +1355,70 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>10</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>10</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>10</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>0</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>50</v>
+      <c r="J15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the some kpi information
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -300,7 +300,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>目前測試兩天沒有任何異狀，安裝流程繼續執行中，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到、License 有誤但是還是可以安裝到結束</t>
+    <t>目前測試四天沒有任何異狀，安裝流程繼續執行中，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到、License 有誤但是還是可以安裝到結束</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,9 +561,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -586,6 +583,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -911,7 +911,7 @@
     <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -946,7 +946,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -977,9 +977,8 @@
       <c r="J2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1013,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1045,9 +1044,8 @@
       <c r="J4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
@@ -1097,7 +1095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1130,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>17</v>
       </c>
@@ -1163,11 +1161,11 @@
       <c r="J8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
@@ -1198,44 +1196,44 @@
       <c r="J9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>1000</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>1000</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18">
         <v>603</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <v>397</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>58</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1245,16 +1243,16 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>1500</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>3000</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <v>2991</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="21">
         <v>5</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1263,12 +1261,11 @@
       <c r="I11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -1278,13 +1275,13 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>1500</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>3000</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>2971</v>
       </c>
       <c r="G12" s="16">
@@ -1296,12 +1293,11 @@
       <c r="I12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1311,17 +1307,17 @@
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>1500</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <f>F13+G13</f>
         <v>831</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="22">
         <v>744</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="23">
         <v>87</v>
       </c>
       <c r="H13" s="5" t="s">
@@ -1330,12 +1326,11 @@
       <c r="I13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1345,16 +1340,16 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>1500</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <v>309</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="22">
         <v>263</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="23">
         <v>46</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -1363,12 +1358,11 @@
       <c r="I14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -1390,7 +1384,7 @@
       <c r="G15" s="7">
         <v>0</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
@@ -1403,7 +1397,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
@@ -1438,8 +1432,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
@@ -1471,8 +1464,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+    <row r="18" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Update the kpi information
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,10 +204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(程式已完成) 等待可用設備</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>同一隻程式跑不同設備 Fail Rate 不同</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -301,6 +297,25 @@
   </si>
   <si>
     <t>目前測試四天沒有任何異狀，安裝流程繼續執行中，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到、License 有誤但是還是可以安裝到結束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USC-130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WLAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試完畢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191206_005722</t>
+  </si>
+  <si>
+    <t>測試中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -372,7 +387,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -426,80 +441,63 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
-      </right>
-      <top style="thin">
+      </left>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <bottom style="medium">
         <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color auto="1"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,7 +507,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -528,64 +526,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,29 +880,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="4" style="4" customWidth="1"/>
+    <col min="6" max="6" width="3.75" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.25" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="40.75" style="5" customWidth="1"/>
     <col min="12" max="12" width="25.5" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -937,7 +925,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>47</v>
@@ -947,73 +935,73 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="13">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="13">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1999</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E3" s="4">
         <v>1000</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F3" s="4">
         <v>994</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G3" s="4">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2000</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1999</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1046,191 +1034,205 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="18">
+        <v>985</v>
+      </c>
+      <c r="G5" s="19">
+        <v>15</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10" t="s">
+      <c r="B6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="21">
         <v>1000</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E6" s="21">
         <v>1000</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="E7" s="7">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7">
+        <v>50</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2000</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="13" t="s">
+      <c r="D8" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1000</v>
+      </c>
+      <c r="F8" s="7">
+        <v>186</v>
+      </c>
+      <c r="G8" s="8">
+        <v>814</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="15">
-        <v>50</v>
-      </c>
-      <c r="E7" s="15">
-        <v>50</v>
-      </c>
-      <c r="F7" s="15">
-        <v>50</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="15" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D9" s="7">
         <v>1000</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E9" s="7">
         <v>1000</v>
       </c>
-      <c r="F8" s="15">
-        <v>186</v>
-      </c>
-      <c r="G8" s="16">
-        <v>814</v>
-      </c>
-      <c r="H8" s="14" t="s">
+      <c r="F9" s="7">
+        <v>979</v>
+      </c>
+      <c r="G9" s="8">
+        <v>21</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="I9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="7">
         <v>1000</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E10" s="7">
         <v>1000</v>
       </c>
-      <c r="F9" s="15">
-        <v>979</v>
-      </c>
-      <c r="G9" s="16">
-        <v>21</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="F10" s="7">
+        <v>603</v>
+      </c>
+      <c r="G10" s="8">
+        <v>397</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="18">
-        <v>1000</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1000</v>
-      </c>
-      <c r="F10" s="18">
-        <v>603</v>
-      </c>
-      <c r="G10" s="19">
-        <v>397</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="K10" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1243,16 +1245,16 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="9">
         <v>1500</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="9">
         <v>3000</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="9">
         <v>2991</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="9">
         <v>5</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1261,7 +1263,7 @@
       <c r="I11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1275,16 +1277,16 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="9">
         <v>1500</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="9">
         <v>3000</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="9">
         <v>2971</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="8">
         <v>29</v>
       </c>
       <c r="H12" s="5" t="s">
@@ -1293,7 +1295,7 @@
       <c r="I12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1307,17 +1309,17 @@
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="9">
         <v>1500</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="10">
         <f>F13+G13</f>
         <v>831</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="10">
         <v>744</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="11">
         <v>87</v>
       </c>
       <c r="H13" s="5" t="s">
@@ -1326,7 +1328,7 @@
       <c r="I13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1340,16 +1342,16 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="9">
         <v>1500</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="10">
         <v>309</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="10">
         <v>263</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="11">
         <v>46</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -1358,7 +1360,7 @@
       <c r="I14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1384,7 +1386,7 @@
       <c r="G15" s="7">
         <v>0</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
@@ -1393,107 +1395,113 @@
       <c r="J15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="E16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="K17" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="5" t="s">
+      <c r="I18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit the android 8.1 for adb testing and statistic
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,74 +248,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows 10 x64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019111_230256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PXE for Legacy x64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191113_092921</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前測試一天沒有任何異狀，安裝流程繼續執行中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191115_092921</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停留在 Windows 進入狀態，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前測試四天沒有任何異狀，安裝流程繼續執行中，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到、License 有誤但是還是可以安裝到結束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USC-130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WLAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試完畢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191206_005722</t>
+  </si>
+  <si>
     <t>Local</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>n/a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Windows 10 x64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019111_230256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PXE for Legacy x64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191113_092921</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目前測試一天沒有任何異狀，安裝流程繼續執行中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PASS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191115_092921</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>停留在 Windows 進入狀態，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目前測試四天沒有任何異狀，安裝流程繼續執行中，WDS 的 Error 說明是 IP 暫時沒抓到但是後面有重新抓到、License 有誤但是還是可以安裝到結束</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USC-130</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WLAN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>測試完畢</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20191206_005722</t>
-  </si>
-  <si>
-    <t>測試中</t>
+    <t>20191206_212749</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,7 +387,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -471,17 +471,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -507,7 +496,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -553,28 +542,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -901,7 +893,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -965,7 +957,7 @@
       <c r="J2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1034,67 +1026,73 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="17">
+        <v>985</v>
+      </c>
+      <c r="G5" s="18">
+        <v>15</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="18">
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="19">
         <v>1000</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E6" s="19">
         <v>1000</v>
       </c>
-      <c r="F5" s="18">
-        <v>985</v>
-      </c>
-      <c r="G5" s="19">
-        <v>15</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="F6" s="19">
+        <v>997</v>
+      </c>
+      <c r="G6" s="22">
+        <v>3</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="21">
-        <v>1000</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="19" t="s">
         <v>78</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1163,7 +1161,7 @@
       <c r="J8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="21" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1198,7 +1196,7 @@
       <c r="J9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1401,7 +1399,7 @@
     </row>
     <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>59</v>
@@ -1410,33 +1408,33 @@
         <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>59</v>
@@ -1445,33 +1443,33 @@
         <v>60</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>59</v>
@@ -1480,28 +1478,28 @@
         <v>60</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="I18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="K18" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the statistics of USC-120 test report
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -387,7 +387,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -417,17 +417,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -490,19 +479,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,46 +557,52 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -876,187 +912,189 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="6.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="3.75" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.25" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16.125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="40.75" style="5" customWidth="1"/>
-    <col min="12" max="12" width="25.5" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="13.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.75" style="3" customWidth="1"/>
+    <col min="7" max="7" width="3.25" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="40.75" style="4" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>2000</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="9">
         <v>2000</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="9">
         <v>1999</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="9">
         <v>1</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1000</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>1000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>994</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1000</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1000</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>998</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="13">
         <v>1000</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <v>1000</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <v>985</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>15</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="10" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1064,441 +1102,445 @@
       <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <v>1000</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="15">
         <v>1000</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <v>997</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="18">
         <v>3</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>50</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>50</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>50</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>1000</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>1000</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>186</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>814</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1000</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>1000</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>979</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>21</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="21"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>1000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>1000</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>603</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>397</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>1500</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>3000</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>2991</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>5</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>1500</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>3000</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>2971</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>29</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>1500</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <f>F13+G13</f>
         <v>831</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>744</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="7">
         <v>87</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>1500</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>309</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <v>263</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="7">
         <v>46</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>10</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>10</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>10</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>0</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="17" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update kpi and program index
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Statistics" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Statistics!$A$1:$O$34</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,10 +294,6 @@
     <t>20191211_170316</t>
   </si>
   <si>
-    <t>For Sikuli Script (測試完畢)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20191214_190937</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -383,10 +382,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>For Cisco AP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cisco</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -442,13 +437,34 @@
   </si>
   <si>
     <t>20191227_133318</t>
+  </si>
+  <si>
+    <t>20191228_012917</t>
+  </si>
+  <si>
+    <t>RT-AC68U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cisco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Sikuli Script</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20191231_081606</t>
+  </si>
+  <si>
+    <t>20191231_135901</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,6 +522,14 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF92D050"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -600,7 +624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -662,6 +686,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -968,16 +998,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="17" customWidth="1"/>
+    <col min="1" max="1" width="9.75" style="17" customWidth="1"/>
     <col min="2" max="2" width="9" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.75" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="17" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="17" customWidth="1"/>
     <col min="5" max="5" width="7.75" style="17" customWidth="1"/>
     <col min="6" max="6" width="8.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="6.25" style="3" customWidth="1"/>
@@ -995,22 +1028,22 @@
   <sheetData>
     <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>31</v>
@@ -1034,30 +1067,30 @@
         <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>15</v>
@@ -1087,7 +1120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1095,16 +1128,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>14</v>
@@ -1131,7 +1164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1139,16 +1172,16 @@
         <v>41</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -1175,7 +1208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
@@ -1183,16 +1216,16 @@
         <v>64</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>65</v>
@@ -1222,7 +1255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
@@ -1230,16 +1263,16 @@
         <v>64</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>14</v>
@@ -1269,24 +1302,24 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -1316,7 +1349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
@@ -1324,16 +1357,16 @@
         <v>17</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>15</v>
@@ -1359,11 +1392,11 @@
       <c r="N8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>8</v>
       </c>
@@ -1371,16 +1404,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>15</v>
@@ -1406,355 +1439,355 @@
       <c r="N9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="21"/>
-    </row>
-    <row r="10" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="O9" s="23"/>
+    </row>
+    <row r="10" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J10" s="6">
+        <v>603</v>
+      </c>
+      <c r="K10" s="5">
+        <v>397</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="C11" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J11" s="6">
+        <v>991</v>
+      </c>
+      <c r="K11" s="5">
+        <v>9</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="15" t="s">
+      <c r="E12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I10" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J10" s="15">
-        <v>991</v>
-      </c>
-      <c r="K10" s="5">
-        <v>9</v>
-      </c>
-      <c r="L10" s="16" t="s">
+      <c r="H12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>993</v>
+      </c>
+      <c r="K12" s="5">
+        <v>7</v>
+      </c>
+      <c r="L12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N10" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="O10" s="16" t="s">
+      <c r="N12" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="O12" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J13" s="6">
+        <v>961</v>
+      </c>
+      <c r="K13" s="5">
+        <v>39</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="C15" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="15" t="s">
+      <c r="G15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I11" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J11" s="15">
-        <v>993</v>
-      </c>
-      <c r="K11" s="5">
-        <v>7</v>
-      </c>
-      <c r="L11" s="16" t="s">
+      <c r="H15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="6">
+        <v>996</v>
+      </c>
+      <c r="K15" s="5">
+        <v>4</v>
+      </c>
+      <c r="L15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="N15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I12" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J12" s="15">
-        <v>961</v>
-      </c>
-      <c r="K12" s="5">
-        <v>39</v>
-      </c>
-      <c r="L12" s="16" t="s">
+      <c r="H16" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="6">
+        <v>956</v>
+      </c>
+      <c r="K16" s="5">
+        <v>44</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I13" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J13" s="15">
-        <v>1000</v>
-      </c>
-      <c r="K13" s="6">
-        <v>0</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I14" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J14" s="15">
-        <v>996</v>
-      </c>
-      <c r="K14" s="5">
-        <v>4</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N14" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I15" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J15" s="15">
-        <v>956</v>
-      </c>
-      <c r="K15" s="5">
-        <v>44</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="15">
-        <v>1000</v>
-      </c>
-      <c r="I16" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J16" s="15">
-        <v>863</v>
-      </c>
-      <c r="K16" s="5">
-        <v>137</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="B17" s="16" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>15</v>
@@ -1765,432 +1798,785 @@
       <c r="I17" s="15">
         <v>1000</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="5"/>
+      <c r="J17" s="15">
+        <v>863</v>
+      </c>
+      <c r="K17" s="5">
+        <v>137</v>
+      </c>
       <c r="L17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="O17" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="15">
+        <v>1000</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N20" s="15"/>
+      <c r="O20" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="17" t="s">
+      <c r="E21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N21" s="15"/>
+      <c r="O21" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I22" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N22" s="15"/>
+      <c r="O22" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J23" s="15">
+        <v>830</v>
+      </c>
+      <c r="K23" s="5">
+        <v>137</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I24" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1000</v>
-      </c>
-      <c r="J18" s="6">
-        <v>603</v>
-      </c>
-      <c r="K18" s="5">
-        <v>397</v>
-      </c>
-      <c r="L18" s="14" t="s">
+      <c r="E25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I25" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J25" s="15"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="M25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="15">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="15">
+        <v>1000</v>
+      </c>
+      <c r="J26" s="15">
+        <v>1000</v>
+      </c>
+      <c r="K26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B27" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="C27" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="G27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I27" s="6">
+        <v>3000</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2991</v>
+      </c>
+      <c r="K27" s="6">
+        <v>5</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="E28" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I28" s="6">
+        <v>3000</v>
+      </c>
+      <c r="J28" s="6">
+        <v>2971</v>
+      </c>
+      <c r="K28" s="5">
+        <v>29</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I29" s="6">
+        <f>J29+K29</f>
+        <v>831</v>
+      </c>
+      <c r="J29" s="6">
+        <v>744</v>
+      </c>
+      <c r="K29" s="5">
         <v>87</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="L29" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I30" s="6">
+        <v>309</v>
+      </c>
+      <c r="J30" s="6">
+        <v>263</v>
+      </c>
+      <c r="K30" s="5">
+        <v>46</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="6">
         <v>10</v>
       </c>
-      <c r="H19" s="6">
-        <v>1500</v>
-      </c>
-      <c r="I19" s="6">
-        <v>3000</v>
-      </c>
-      <c r="J19" s="6">
-        <v>2991</v>
-      </c>
-      <c r="K19" s="6">
-        <v>5</v>
-      </c>
-      <c r="L19" s="14" t="s">
+      <c r="I31" s="6">
+        <v>10</v>
+      </c>
+      <c r="J31" s="6">
+        <v>10</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="M31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="6">
-        <v>1500</v>
-      </c>
-      <c r="I20" s="6">
-        <v>3000</v>
-      </c>
-      <c r="J20" s="6">
-        <v>2971</v>
-      </c>
-      <c r="K20" s="5">
-        <v>29</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="14" t="s">
+      <c r="N32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1500</v>
-      </c>
-      <c r="I21" s="6">
-        <f>J21+K21</f>
-        <v>831</v>
-      </c>
-      <c r="J21" s="6">
-        <v>744</v>
-      </c>
-      <c r="K21" s="5">
+      <c r="N33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O33" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="77.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="L21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="6">
-        <v>1500</v>
-      </c>
-      <c r="I22" s="6">
-        <v>309</v>
-      </c>
-      <c r="J22" s="6">
-        <v>263</v>
-      </c>
-      <c r="K22" s="5">
-        <v>46</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="6">
-        <v>10</v>
-      </c>
-      <c r="I23" s="6">
-        <v>10</v>
-      </c>
-      <c r="J23" s="6">
-        <v>10</v>
-      </c>
-      <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O24" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N26" s="3" t="s">
+      <c r="N34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O26" s="17" t="s">
+      <c r="O34" s="17" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O34">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="airplane_wlan_windows_sikuli"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="O8:O9"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update the Statistics and plum.sqlit
</commit_message>
<xml_diff>
--- a/kpi/Statistics.xlsx
+++ b/kpi/Statistics.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Statistics" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Statistics!$A$1:$O$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Statistics!$A$1:$O$50</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="150">
   <si>
     <t>Cycle Times</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -517,33 +517,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sikuli</t>
-  </si>
-  <si>
-    <t>Sikuli</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sikuli</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sikuli</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sikuli, arp -d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DIR-615</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sikuli, arp -d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20200109_094542</t>
   </si>
   <si>
@@ -551,6 +528,58 @@
   </si>
   <si>
     <t>Sierra Wireless EM7455</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join arp -d, Time.sleep, Ping check, Sikuli API wait</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join Sikuli API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join Sikuli API, Time.sleep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join Sikuli API, Time.sleep, Join arp -d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200115_163815</t>
+  </si>
+  <si>
+    <t>20200115_194512</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xiaomi_31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200116_014436</t>
+  </si>
+  <si>
+    <t>20200115_212458</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xiaomi_32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200115_225039</t>
+  </si>
+  <si>
+    <t>Join arp -d, Time.sleep, Ping check, Sikuli API wait, clean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join arp -d, Time.sleep, Ping check, Sikuli API wait, clean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -638,7 +667,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -712,13 +741,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -785,10 +885,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1096,7 +1229,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -1104,9 +1237,8 @@
   <cols>
     <col min="1" max="1" width="9.75" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="16" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="13.25" style="16" customWidth="1"/>
+    <col min="4" max="5" width="10.5" style="16" customWidth="1"/>
     <col min="6" max="6" width="8.125" style="16" customWidth="1"/>
     <col min="7" max="7" width="6.25" style="3" customWidth="1"/>
     <col min="8" max="8" width="4.625" style="3" customWidth="1"/>
@@ -1116,7 +1248,7 @@
     <col min="12" max="12" width="23.625" style="3" customWidth="1"/>
     <col min="13" max="13" width="20.25" style="3" customWidth="1"/>
     <col min="14" max="14" width="12.625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="27.5" style="21" customWidth="1"/>
+    <col min="15" max="15" width="36" style="21" customWidth="1"/>
     <col min="16" max="16" width="25.5" style="3" customWidth="1"/>
     <col min="17" max="16384" width="9" style="3"/>
   </cols>
@@ -1211,7 +1343,7 @@
       <c r="N2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1487,7 +1619,7 @@
       <c r="N8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="35" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1534,7 +1666,7 @@
       <c r="N9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="24"/>
+      <c r="O9" s="35"/>
     </row>
     <row r="10" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1807,7 +1939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>56</v>
       </c>
@@ -1992,7 +2124,7 @@
         <v>69</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
@@ -2039,7 +2171,7 @@
         <v>70</v>
       </c>
       <c r="O20" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2086,7 +2218,7 @@
         <v>71</v>
       </c>
       <c r="O21" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2133,7 +2265,7 @@
         <v>74</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
@@ -2180,7 +2312,7 @@
         <v>75</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2227,7 +2359,7 @@
         <v>76</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2274,7 +2406,7 @@
         <v>105</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2321,575 +2453,1097 @@
         <v>106</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="D27" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I27" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J27" s="14">
+      <c r="H27" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J27" s="6">
         <v>650</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="6">
         <v>350</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="L27" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="N27" s="6" t="s">
         <v>112</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="15" t="s">
+      <c r="D28" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I28" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J28" s="14">
+      <c r="H28" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I28" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J28" s="6">
         <v>998</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="6">
         <v>2</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="N28" s="6" t="s">
         <v>116</v>
       </c>
       <c r="O28" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:15" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" s="15" t="s">
+      <c r="D29" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I29" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J29" s="14">
+      <c r="H29" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J29" s="6">
         <v>990</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="6">
         <v>10</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N29" s="14" t="s">
+      <c r="N29" s="6" t="s">
         <v>113</v>
       </c>
       <c r="O29" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="D30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I30" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J30" s="14">
+      <c r="H30" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I30" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J30" s="6">
         <v>1000</v>
       </c>
       <c r="K30" s="6">
         <v>0</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="M30" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N30" s="14" t="s">
+      <c r="N30" s="6" t="s">
         <v>111</v>
       </c>
       <c r="O30" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="15" t="s">
+      <c r="D31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I31" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J31" s="14">
+      <c r="H31" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J31" s="6">
         <v>830</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="6">
         <v>137</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="M31" s="14" t="s">
+      <c r="M31" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="N31" s="6" t="s">
         <v>108</v>
       </c>
       <c r="O31" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="15" t="s">
+      <c r="D32" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I32" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J32" s="14">
+      <c r="H32" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I32" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J32" s="6">
         <v>999</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="6">
         <v>1</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="6" t="s">
         <v>110</v>
       </c>
       <c r="O32" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="15" t="s">
+      <c r="E33" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I33" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J33" s="14">
+      <c r="H33" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I33" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J33" s="6">
         <v>991</v>
       </c>
-      <c r="K33" s="5">
+      <c r="K33" s="6">
         <v>9</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N33" s="14" t="s">
+      <c r="N33" s="6" t="s">
         <v>109</v>
       </c>
       <c r="O33" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="D34" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I34" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J34" s="14">
+      <c r="H34" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I34" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J34" s="6">
         <v>1000</v>
       </c>
       <c r="K34" s="6">
         <v>0</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="M34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N34" s="14" t="s">
+      <c r="N34" s="6" t="s">
         <v>107</v>
       </c>
       <c r="O34" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I35" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J35" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="O35" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J36" s="6">
+        <v>366</v>
+      </c>
+      <c r="K36" s="6">
+        <v>634</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="O36" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="24" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="G37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="25">
+        <v>1000</v>
+      </c>
+      <c r="I37" s="25">
+        <v>1000</v>
+      </c>
+      <c r="J37" s="25">
+        <v>349</v>
+      </c>
+      <c r="K37" s="26">
+        <v>651</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="M37" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="O37" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="32">
+        <v>1000</v>
+      </c>
+      <c r="I38" s="32">
+        <v>1000</v>
+      </c>
+      <c r="J38" s="32">
+        <v>909</v>
+      </c>
+      <c r="K38" s="33">
+        <v>91</v>
+      </c>
+      <c r="L38" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="M38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="N38" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="O38" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="25">
+        <v>1000</v>
+      </c>
+      <c r="I39" s="25">
+        <v>1000</v>
+      </c>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N39" s="25"/>
+      <c r="O39" s="27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I40" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M40" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N40" s="14"/>
+      <c r="O40" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I41" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M41" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N41" s="14"/>
+      <c r="O41" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B42" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C42" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G35" s="14" t="s">
+      <c r="D42" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I35" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J35" s="14">
-        <v>1000</v>
-      </c>
-      <c r="K35" s="3">
+      <c r="H42" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I42" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M42" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N42" s="14"/>
+      <c r="O42" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I43" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M43" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N43" s="14"/>
+      <c r="O43" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="32">
+        <v>1000</v>
+      </c>
+      <c r="I44" s="32">
+        <v>1000</v>
+      </c>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="M44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="N44" s="32"/>
+      <c r="O44" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="25">
+        <v>1000</v>
+      </c>
+      <c r="I45" s="25">
+        <v>1000</v>
+      </c>
+      <c r="J45" s="25">
+        <v>1000</v>
+      </c>
+      <c r="K45" s="25">
         <v>0</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="L45" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M45" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N45" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="O45" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I46" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J46" s="14">
+        <v>1000</v>
+      </c>
+      <c r="K46" s="14">
+        <v>0</v>
+      </c>
+      <c r="L46" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M46" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N46" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="O46" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I47" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J47" s="14">
+        <v>1000</v>
+      </c>
+      <c r="K47" s="14">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M47" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N47" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="O47" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I48" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J48" s="14">
+        <v>1000</v>
+      </c>
+      <c r="K48" s="14">
+        <v>0</v>
+      </c>
+      <c r="L48" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="14" t="s">
+      <c r="M48" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N35" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="O35" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="N48" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="O48" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B49" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C49" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G36" s="14" t="s">
+      <c r="D49" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I36" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J36" s="14">
-        <v>366</v>
-      </c>
-      <c r="K36" s="5">
-        <v>634</v>
-      </c>
-      <c r="L36" s="15" t="s">
+      <c r="H49" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I49" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J49" s="14">
+        <v>1000</v>
+      </c>
+      <c r="K49" s="14">
+        <v>0</v>
+      </c>
+      <c r="L49" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="M36" s="14" t="s">
+      <c r="M49" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N36" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O36" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="N49" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="O49" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B50" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C50" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G37" s="14" t="s">
+      <c r="D50" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="G50" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I37" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J37" s="14">
-        <v>349</v>
-      </c>
-      <c r="K37" s="5">
-        <v>651</v>
-      </c>
-      <c r="L37" s="15" t="s">
+      <c r="H50" s="32">
+        <v>1000</v>
+      </c>
+      <c r="I50" s="32">
+        <v>1000</v>
+      </c>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="M37" s="14" t="s">
+      <c r="M50" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="N37" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="O37" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I38" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J38" s="14">
-        <v>909</v>
-      </c>
-      <c r="K38" s="5">
-        <v>91</v>
-      </c>
-      <c r="L38" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="M38" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="N38" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="O38" s="13" t="s">
-        <v>136</v>
+      <c r="N50" s="32"/>
+      <c r="O50" s="29" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O37">
+  <autoFilter ref="A1:O50">
     <filterColumn colId="12">
       <filters>
         <filter val="airplane_wlan_windows_sikuli"/>

</xml_diff>